<commit_message>
New test cases add
</commit_message>
<xml_diff>
--- a/OrangeHRM.xlsx
+++ b/OrangeHRM.xlsx
@@ -5,17 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1c57d86eb9cd3963/Desktop/SoftwareTesting/ManualTestingProjects/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pooja\OneDrive\Desktop\SoftwareTesting\ManualTestingProjects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="8_{FCE7BAA6-40FA-403A-9DEC-2CE4414D98CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECEF3171-865E-4708-843D-8C90BB7B75C0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6064DCD2-714A-4603-A176-0290EBDF0462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{369F12F9-A5E4-4297-A44E-5F75D8CCD4F1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{369F12F9-A5E4-4297-A44E-5F75D8CCD4F1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Test_Scenario" sheetId="1" r:id="rId1"/>
-    <sheet name="Login_Dashboard_Test_cases" sheetId="2" r:id="rId2"/>
-    <sheet name="PIM_Module" sheetId="3" r:id="rId3"/>
+    <sheet name="Project Details" sheetId="4" r:id="rId1"/>
+    <sheet name="Desicion_table" sheetId="5" r:id="rId2"/>
+    <sheet name="Test_Scenario" sheetId="1" r:id="rId3"/>
+    <sheet name="Login_Dashboard_Test_cases" sheetId="2" r:id="rId4"/>
+    <sheet name="PIM_Module" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="161">
   <si>
     <t>Test Scenario TID</t>
   </si>
@@ -98,40 +100,16 @@
     <t>TC_001</t>
   </si>
   <si>
-    <t>Login with valid credentials</t>
-  </si>
-  <si>
-    <t>1. Enter username Admin
-2. Enter password admin123
-3. Click Login button</t>
-  </si>
-  <si>
     <t>User is redirected to dashboard</t>
   </si>
   <si>
     <t>TC_002</t>
   </si>
   <si>
-    <t>Login with invalid username</t>
-  </si>
-  <si>
     <t>User is on Login page</t>
   </si>
   <si>
-    <t>1. Enter invalid username WrongUser
-2. Enter valid password admin123
-3. Click Login button</t>
-  </si>
-  <si>
     <t>Error: Invalid credentials</t>
-  </si>
-  <si>
-    <t>Login with invalid password</t>
-  </si>
-  <si>
-    <t>1. Enter valid username Admin
-2. Enter wrong password wrong123
-3. Click Login button</t>
   </si>
   <si>
     <t>Attempt login with both fields blank</t>
@@ -530,12 +508,217 @@
   <si>
     <t>Pooja</t>
   </si>
+  <si>
+    <t>Project Details</t>
+  </si>
+  <si>
+    <t>Project Name</t>
+  </si>
+  <si>
+    <t>Module Name</t>
+  </si>
+  <si>
+    <t>Assign date</t>
+  </si>
+  <si>
+    <t>Assign By</t>
+  </si>
+  <si>
+    <t>Browser version</t>
+  </si>
+  <si>
+    <t>Build No</t>
+  </si>
+  <si>
+    <t>Cross browser testing</t>
+  </si>
+  <si>
+    <t>OrangeHRMLive</t>
+  </si>
+  <si>
+    <t>Login and PIM</t>
+  </si>
+  <si>
+    <t>QA Lead(Sagar Ambi)</t>
+  </si>
+  <si>
+    <t>135.0.7049.117</t>
+  </si>
+  <si>
+    <t>1.0.1</t>
+  </si>
+  <si>
+    <t>Cgrome | Edge</t>
+  </si>
+  <si>
+    <t>Decision Table</t>
+  </si>
+  <si>
+    <t>Fields</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Outcomes</t>
+  </si>
+  <si>
+    <t>TC1</t>
+  </si>
+  <si>
+    <t>TC2</t>
+  </si>
+  <si>
+    <t>TC3</t>
+  </si>
+  <si>
+    <t>TC4</t>
+  </si>
+  <si>
+    <t>TC5</t>
+  </si>
+  <si>
+    <t>TC6</t>
+  </si>
+  <si>
+    <t>TC7</t>
+  </si>
+  <si>
+    <t>TC8</t>
+  </si>
+  <si>
+    <t>TC9</t>
+  </si>
+  <si>
+    <t>Valid</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>Invalid</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <r>
+      <t>Test Scenario(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>OrangeHRM live</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>TC_019</t>
+  </si>
+  <si>
+    <t>TC_020</t>
+  </si>
+  <si>
+    <t>TC_021</t>
+  </si>
+  <si>
+    <t>TC_022</t>
+  </si>
+  <si>
+    <t>Login with invalid username and valid password.</t>
+  </si>
+  <si>
+    <t>Login with valid credentials.</t>
+  </si>
+  <si>
+    <t>Login with valid username and invalid password.</t>
+  </si>
+  <si>
+    <t>Login with invalid password and invalid username.</t>
+  </si>
+  <si>
+    <t>1. Enter invalid username.
+2. Enter invalid password.
+3. Click Login button</t>
+  </si>
+  <si>
+    <t>1. Enter valid username.
+2. Enter wrong password.
+3. Click Login button</t>
+  </si>
+  <si>
+    <t>1. Enter invalid username.
+2. Enter valid password.
+3. Click Login button</t>
+  </si>
+  <si>
+    <t>1. Enter username Admin.
+2. Enter password admin123.
+3. Click Login button</t>
+  </si>
+  <si>
+    <t>Login with valid username and blanck password.</t>
+  </si>
+  <si>
+    <t>Login with Blank username and valid password.</t>
+  </si>
+  <si>
+    <t>Login with invalid username and blanck password.</t>
+  </si>
+  <si>
+    <t>TC_023</t>
+  </si>
+  <si>
+    <t>1. Enter valid username.
+2. Enter blanck password.
+3. Click Login button</t>
+  </si>
+  <si>
+    <t>1. Enter blanck username.
+2. Enter valid password.
+3. Click Login button</t>
+  </si>
+  <si>
+    <t>1. Enter invalid username.
+2. Enter blanck password.
+3. Click Login button</t>
+  </si>
+  <si>
+    <t>1. Enter blanck username.
+2. Enter invalid password.
+3. Click Login button</t>
+  </si>
+  <si>
+    <t>Login with blanck username and invalid password.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -567,8 +750,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -579,6 +778,24 @@
       <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -609,7 +826,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -628,6 +845,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -942,90 +1174,377 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF44B03-476A-425F-9AD3-E4F49F08376E}">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93AF016A-5912-4190-A7D3-1610244A4E64}">
+  <dimension ref="B1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B1" sqref="B1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="3" max="3" width="22.21875" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" customWidth="1"/>
+    <col min="5" max="5" width="32.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B2" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" s="8">
+        <v>45784</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CD5B327-0517-4407-983C-C69CFE23723F}">
+  <dimension ref="A1:J26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+    </row>
+    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+    </row>
+    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="26" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J26" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:J1"/>
+  </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF44B03-476A-425F-9AD3-E4F49F08376E}">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34.5546875" customWidth="1"/>
-    <col min="2" max="2" width="45" customWidth="1"/>
+    <col min="2" max="2" width="35.88671875" customWidth="1"/>
     <col min="3" max="3" width="26.77734375" customWidth="1"/>
     <col min="4" max="4" width="24.109375" customWidth="1"/>
     <col min="5" max="5" width="34.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.45">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:5" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+    </row>
+    <row r="3" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.45">
+      <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1">
-        <v>10</v>
-      </c>
-      <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1">
+        <v>8</v>
+      </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="10" spans="1:5" ht="21.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="12" spans="1:5" ht="21.6" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5FA13AB-753F-4608-9F5C-26FBA23DE275}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1089,27 +1608,27 @@
         <v>19</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="H2" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="6" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="K2" s="3"/>
     </row>
-    <row r="3" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -1117,30 +1636,30 @@
         <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="H3" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="6" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -1148,26 +1667,26 @@
         <v>6</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>28</v>
+        <v>146</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>29</v>
+        <v>149</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="6" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="K4" s="3"/>
     </row>
@@ -1179,30 +1698,28 @@
         <v>6</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>31</v>
+        <v>148</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>110</v>
+        <v>23</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>110</v>
+        <v>23</v>
       </c>
       <c r="I5" s="3"/>
-      <c r="J5" s="6" t="s">
-        <v>111</v>
-      </c>
+      <c r="J5" s="6"/>
       <c r="K5" s="3"/>
     </row>
-    <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -1210,30 +1727,28 @@
         <v>6</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>32</v>
+        <v>152</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>33</v>
+        <v>156</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="I6" s="3"/>
-      <c r="J6" s="6" t="s">
-        <v>111</v>
-      </c>
+      <c r="J6" s="6"/>
       <c r="K6" s="3"/>
     </row>
-    <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1241,30 +1756,28 @@
         <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>35</v>
+        <v>153</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>36</v>
+        <v>157</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="I7" s="3"/>
-      <c r="J7" s="6" t="s">
-        <v>111</v>
-      </c>
+      <c r="J7" s="6"/>
       <c r="K7" s="3"/>
     </row>
-    <row r="8" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
@@ -1272,30 +1785,28 @@
         <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>38</v>
+        <v>154</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>39</v>
+        <v>158</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="I8" s="3"/>
-      <c r="J8" s="6" t="s">
-        <v>111</v>
-      </c>
+      <c r="J8" s="6"/>
       <c r="K8" s="3"/>
     </row>
-    <row r="9" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
@@ -1303,327 +1814,480 @@
         <v>6</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>41</v>
+        <v>160</v>
       </c>
       <c r="E9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" s="3"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="I9" s="3"/>
-      <c r="J9" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="K9" s="3"/>
-    </row>
-    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="G10" s="3" t="s">
-        <v>57</v>
+        <v>104</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="I10" s="4"/>
+        <v>104</v>
+      </c>
+      <c r="I10" s="3"/>
       <c r="J10" s="6" t="s">
-        <v>111</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="K10" s="3"/>
     </row>
     <row r="11" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>78</v>
+        <v>28</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="I11" s="4"/>
+        <v>28</v>
+      </c>
+      <c r="I11" s="3"/>
       <c r="J11" s="6" t="s">
-        <v>111</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="K11" s="3"/>
     </row>
     <row r="12" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>79</v>
+        <v>31</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="I12" s="4"/>
+        <v>31</v>
+      </c>
+      <c r="I12" s="3"/>
       <c r="J12" s="6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>79</v>
+        <v>34</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="I13" s="4"/>
+        <v>23</v>
+      </c>
+      <c r="I13" s="3"/>
       <c r="J13" s="6" t="s">
-        <v>111</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="K13" s="3"/>
     </row>
     <row r="14" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>79</v>
+        <v>37</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="I14" s="4"/>
+        <v>37</v>
+      </c>
+      <c r="I14" s="3"/>
       <c r="J14" s="6" t="s">
-        <v>111</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="K14" s="3"/>
     </row>
     <row r="15" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="6" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>63</v>
-      </c>
       <c r="E16" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="6" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C18" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>79</v>
-      </c>
       <c r="H18" s="3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
-        <v>44</v>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I19" s="4"/>
       <c r="J19" s="6" t="s">
-        <v>111</v>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I20" s="4"/>
+      <c r="J20" s="6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I21" s="4"/>
+      <c r="J21" s="6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I22" s="4"/>
+      <c r="J22" s="6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I23" s="4"/>
+      <c r="J23" s="6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I24" s="4"/>
+      <c r="J24" s="6" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1632,11 +2296,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6325E384-6171-4048-AC05-FAB61936DC79}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -1692,187 +2356,187 @@
     </row>
     <row r="2" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="6" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>90</v>
-      </c>
       <c r="H3" s="3" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="6" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="6" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="6" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="K5" s="3"/>
     </row>
     <row r="6" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>104</v>
-      </c>
       <c r="H6" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="6" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="K6" s="3"/>
     </row>
     <row r="7" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="6" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="K7" s="3"/>
     </row>

</xml_diff>